<commit_message>
Updates for night of the big wind
</commit_message>
<xml_diff>
--- a/night-big-wind/rough-locations.xlsx
+++ b/night-big-wind/rough-locations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ed/Documents/GitHub/weather-rescue/night-big-wind/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4A1247-8C5F-3A4E-8EA5-2B1D2C1C7EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951087B0-A4F4-4342-B278-FC9CEC9BAA33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="500" windowWidth="10000" windowHeight="16940" xr2:uid="{956636CC-2F8C-EF47-81E6-ADBD09CAFC15}"/>
+    <workbookView xWindow="4120" yWindow="3660" windowWidth="13900" windowHeight="16940" xr2:uid="{956636CC-2F8C-EF47-81E6-ADBD09CAFC15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Armagh</t>
   </si>
@@ -128,6 +128,30 @@
   </si>
   <si>
     <t>Carbeth</t>
+  </si>
+  <si>
+    <t>Ballimore</t>
+  </si>
+  <si>
+    <t>Kendal</t>
+  </si>
+  <si>
+    <t>Epping</t>
+  </si>
+  <si>
+    <t>Castle Cary</t>
+  </si>
+  <si>
+    <t>Benefield</t>
+  </si>
+  <si>
+    <t>Aylesbury</t>
+  </si>
+  <si>
+    <t>Trumpington</t>
+  </si>
+  <si>
+    <t>Guilsborough</t>
   </si>
 </sst>
 </file>
@@ -479,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA6576C-B8C9-5B4D-B110-95EB9DA3F436}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -833,6 +857,94 @@
         <v>-4.37</v>
       </c>
     </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>56</v>
+      </c>
+      <c r="C32">
+        <v>-5.33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>54.33</v>
+      </c>
+      <c r="C33">
+        <v>-2.75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>51.7</v>
+      </c>
+      <c r="C34">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35">
+        <v>52.35</v>
+      </c>
+      <c r="C35">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>51.09</v>
+      </c>
+      <c r="C36">
+        <v>-2.5099999999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>52.48</v>
+      </c>
+      <c r="C37">
+        <v>-0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>52.82</v>
+      </c>
+      <c r="C38">
+        <v>-0.81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>52.17</v>
+      </c>
+      <c r="C39">
+        <v>0.11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update to night of the big wind
</commit_message>
<xml_diff>
--- a/night-big-wind/rough-locations.xlsx
+++ b/night-big-wind/rough-locations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ed/Documents/GitHub/weather-rescue/night-big-wind/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3936727E-4B13-A94F-A490-3478992BBB8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3708D638-B11F-6C47-82B9-E5CCAD4E6362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9540" yWindow="600" windowWidth="22380" windowHeight="16940" xr2:uid="{956636CC-2F8C-EF47-81E6-ADBD09CAFC15}"/>
+    <workbookView xWindow="6640" yWindow="3040" windowWidth="22380" windowHeight="11680" xr2:uid="{956636CC-2F8C-EF47-81E6-ADBD09CAFC15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
   <si>
     <t>Armagh</t>
   </si>
@@ -228,6 +228,39 @@
   </si>
   <si>
     <t>Neath</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Herisau</t>
+  </si>
+  <si>
+    <t>Bern</t>
+  </si>
+  <si>
+    <t>Bern Trechsel</t>
+  </si>
+  <si>
+    <t>Fribourg</t>
+  </si>
+  <si>
+    <t>Nufenen</t>
+  </si>
+  <si>
+    <t>St Gallen</t>
+  </si>
+  <si>
+    <t>Schaffhausen</t>
+  </si>
+  <si>
+    <t>Vevey</t>
+  </si>
+  <si>
+    <t>Zurich</t>
+  </si>
+  <si>
+    <t>Rovereto</t>
   </si>
 </sst>
 </file>
@@ -292,7 +325,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -580,7 +613,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -588,10 +621,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA6576C-B8C9-5B4D-B110-95EB9DA3F436}">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1622,6 +1656,210 @@
         <v>2</v>
       </c>
     </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>64</v>
+      </c>
+      <c r="B61">
+        <v>52.52</v>
+      </c>
+      <c r="C61">
+        <v>13.4</v>
+      </c>
+      <c r="D61">
+        <v>3</v>
+      </c>
+      <c r="E61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>65</v>
+      </c>
+      <c r="B62">
+        <v>47.384999999999998</v>
+      </c>
+      <c r="C62">
+        <v>9.2789999999999999</v>
+      </c>
+      <c r="D62">
+        <v>3</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>66</v>
+      </c>
+      <c r="B63">
+        <v>46.948</v>
+      </c>
+      <c r="C63">
+        <v>7.452</v>
+      </c>
+      <c r="D63">
+        <v>2</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>67</v>
+      </c>
+      <c r="B64">
+        <v>46.947000000000003</v>
+      </c>
+      <c r="C64">
+        <v>7.4509999999999996</v>
+      </c>
+      <c r="D64">
+        <v>4</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>68</v>
+      </c>
+      <c r="B65">
+        <v>46.807000000000002</v>
+      </c>
+      <c r="C65">
+        <v>7.1580000000000004</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>69</v>
+      </c>
+      <c r="B66">
+        <v>46.539499999999997</v>
+      </c>
+      <c r="C66">
+        <v>9.2439999999999998</v>
+      </c>
+      <c r="D66">
+        <v>3</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>70</v>
+      </c>
+      <c r="B67">
+        <v>47.423999999999999</v>
+      </c>
+      <c r="C67">
+        <v>9.3780000000000001</v>
+      </c>
+      <c r="D67">
+        <v>4</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>71</v>
+      </c>
+      <c r="B68">
+        <v>47.695999999999998</v>
+      </c>
+      <c r="C68">
+        <v>8.6389999999999993</v>
+      </c>
+      <c r="D68">
+        <v>3</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>72</v>
+      </c>
+      <c r="B69">
+        <v>46.46</v>
+      </c>
+      <c r="C69">
+        <v>6.84</v>
+      </c>
+      <c r="D69">
+        <v>2</v>
+      </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>73</v>
+      </c>
+      <c r="B70">
+        <v>47.37</v>
+      </c>
+      <c r="C70">
+        <v>8.4740000000000002</v>
+      </c>
+      <c r="D70">
+        <v>4</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>53</v>
+      </c>
+      <c r="B71">
+        <v>47.55</v>
+      </c>
+      <c r="C71">
+        <v>7.5910000000000002</v>
+      </c>
+      <c r="D71">
+        <v>5</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>74</v>
+      </c>
+      <c r="B72">
+        <v>45.883000000000003</v>
+      </c>
+      <c r="C72">
+        <v>11.05</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
night big wind updates
</commit_message>
<xml_diff>
--- a/night-big-wind/rough-locations.xlsx
+++ b/night-big-wind/rough-locations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ed/Documents/GitHub/weather-rescue/night-big-wind/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386FFB94-0D78-BE4A-8579-EA02974CED56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8DC0450-66C2-2740-8B9C-C4E8E7235A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="580" windowWidth="10000" windowHeight="11680" xr2:uid="{956636CC-2F8C-EF47-81E6-ADBD09CAFC15}"/>
+    <workbookView xWindow="940" yWindow="580" windowWidth="21480" windowHeight="13660" xr2:uid="{956636CC-2F8C-EF47-81E6-ADBD09CAFC15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="103">
   <si>
     <t>Armagh</t>
   </si>
@@ -342,6 +342,9 @@
   </si>
   <si>
     <t>Start Point (Orkney)</t>
+  </si>
+  <si>
+    <t>Liverpool</t>
   </si>
 </sst>
 </file>
@@ -392,8 +395,125 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="15">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB8AC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFB8AC"/>
+      <color rgb="FFFF988A"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -702,11 +822,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA6576C-B8C9-5B4D-B110-95EB9DA3F436}">
-  <dimension ref="A1:E99"/>
+  <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C87" sqref="C87"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D105" sqref="D105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1173,7 +1293,7 @@
         <v>2</v>
       </c>
       <c r="E27">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -2400,7 +2520,41 @@
         <v>4</v>
       </c>
     </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>102</v>
+      </c>
+      <c r="B100">
+        <v>53.405000000000001</v>
+      </c>
+      <c r="C100">
+        <v>-2.988</v>
+      </c>
+      <c r="D100">
+        <v>2</v>
+      </c>
+      <c r="E100">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+      <formula>"2$B$8"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Additions to night of the big wind
</commit_message>
<xml_diff>
--- a/night-big-wind/rough-locations.xlsx
+++ b/night-big-wind/rough-locations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ed/Documents/GitHub/weather-rescue/night-big-wind/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E8B947-0B6A-934B-8581-C8FA256D0347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9BED299-7FB4-0347-B4ED-0E5DF8322821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3640" yWindow="2480" windowWidth="21480" windowHeight="13660" xr2:uid="{956636CC-2F8C-EF47-81E6-ADBD09CAFC15}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="109">
   <si>
     <t>Armagh</t>
   </si>
@@ -360,6 +360,9 @@
   </si>
   <si>
     <t>London (Greenwich)</t>
+  </si>
+  <si>
+    <t>Allenheads</t>
   </si>
 </sst>
 </file>
@@ -763,11 +766,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA6576C-B8C9-5B4D-B110-95EB9DA3F436}">
-  <dimension ref="A1:E105"/>
+  <dimension ref="A1:E106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
+      <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2560,6 +2563,23 @@
         <v>4</v>
       </c>
       <c r="E105">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>108</v>
+      </c>
+      <c r="B106">
+        <v>54.8</v>
+      </c>
+      <c r="C106">
+        <v>-2.2200000000000002</v>
+      </c>
+      <c r="D106">
+        <v>2</v>
+      </c>
+      <c r="E106">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Belgium data, and updates to night of the big wind
</commit_message>
<xml_diff>
--- a/night-big-wind/rough-locations.xlsx
+++ b/night-big-wind/rough-locations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ed/Documents/GitHub/weather-rescue/night-big-wind/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D52A307-B919-3749-B8D0-6BC8960E8D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D454D57-EDEF-224F-B293-E7AF47E8B22F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1240" yWindow="760" windowWidth="21480" windowHeight="13660" xr2:uid="{956636CC-2F8C-EF47-81E6-ADBD09CAFC15}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="119">
   <si>
     <t>Armagh</t>
   </si>
@@ -390,6 +390,9 @@
   </si>
   <si>
     <t>Trondheim</t>
+  </si>
+  <si>
+    <t>Touiouse</t>
   </si>
 </sst>
 </file>
@@ -793,11 +796,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA6576C-B8C9-5B4D-B110-95EB9DA3F436}">
-  <dimension ref="A1:E114"/>
+  <dimension ref="A1:E115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G105" sqref="G105"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D109" sqref="D109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2744,6 +2747,23 @@
       </c>
       <c r="E114">
         <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>118</v>
+      </c>
+      <c r="B115">
+        <v>43.6</v>
+      </c>
+      <c r="C115">
+        <v>1.46</v>
+      </c>
+      <c r="D115">
+        <v>1</v>
+      </c>
+      <c r="E115">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>